<commit_message>
gewichte anpassung so gut wie fertig implementiert
</commit_message>
<xml_diff>
--- a/openEAR-0.1.0 Kopie/GUI/Default Weights/default_weights.xlsx
+++ b/openEAR-0.1.0 Kopie/GUI/Default Weights/default_weights.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Pitch-Session</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Gespräch</t>
   </si>
   <si>
+    <t>Benutzerdefiniert</t>
+  </si>
+  <si>
     <t>w_emodb_anger</t>
   </si>
   <si>
@@ -54,6 +57,9 @@
   </si>
   <si>
     <t>w_abc_nervous</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
   <si>
     <t>w_abc_neutral</t>
@@ -92,7 +98,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -130,7 +136,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -157,49 +170,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,192 +555,243 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="20" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="21" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="22" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="26.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="D4" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="3" t="s">
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
+        <v>8</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10">
+        <v>98</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="C13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="C15" s="10"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13">
+        <v>99</v>
+      </c>
+      <c r="D16" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <v>99</v>
+      </c>
+      <c r="D17" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="C18" s="13">
+        <v>9</v>
+      </c>
+      <c r="D18" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="15">
+        <v>3</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="18">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6">
-        <v>3</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="8">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10">
-        <v>3</v>
-      </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12">
-        <v>1</v>
-      </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
unfertig!!! Live Pie Chart
</commit_message>
<xml_diff>
--- a/openEAR-0.1.0 Kopie/GUI/Default Weights/default_weights.xlsx
+++ b/openEAR-0.1.0 Kopie/GUI/Default Weights/default_weights.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Pitch-Session</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>w_abc_nervous</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>w_abc_neutral</t>
@@ -595,7 +592,9 @@
       <c r="C3" s="7">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5" t="s">
@@ -607,7 +606,9 @@
       <c r="C4" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5" t="s">
@@ -619,7 +620,9 @@
       <c r="C5" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5" t="s">
@@ -631,7 +634,9 @@
       <c r="C6" s="7">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5" t="s">
@@ -643,7 +648,9 @@
       <c r="C7" s="7">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5" t="s">
@@ -655,7 +662,9 @@
       <c r="C8" s="7">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5" t="s">
@@ -667,7 +676,9 @@
       <c r="C9" s="7">
         <v>7</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="8" t="s">
@@ -679,7 +690,9 @@
       <c r="C10" s="10">
         <v>8</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="8" t="s">
@@ -691,7 +704,9 @@
       <c r="C11" s="10">
         <v>98</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
@@ -703,7 +718,9 @@
       <c r="C12" s="10">
         <v>9</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="8" t="s">
@@ -712,34 +729,44 @@
       <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="C13" s="10">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="9">
         <v>4</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="9">
         <v>3</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="10">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="12">
         <v>1</v>
@@ -747,11 +774,13 @@
       <c r="C16" s="13">
         <v>99</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="12">
         <v>1</v>
@@ -759,11 +788,13 @@
       <c r="C17" s="13">
         <v>99</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="12">
         <v>2</v>
@@ -771,27 +802,37 @@
       <c r="C18" s="13">
         <v>9</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="15">
         <v>3</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="16">
+        <v>2</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="18">
         <v>1</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="19">
+        <v>3</v>
+      </c>
+      <c r="D20" s="19">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>